<commit_message>
lr: update oias forms.
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Liberia/lr_oncho_ias_2_participant_202112.xlsx
+++ b/ONCHO/Impact Assessments/Liberia/lr_oncho_ias_2_participant_202112.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="119">
   <si>
     <t>type</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>Enter the age in years</t>
+  </si>
+  <si>
+    <t>. &gt;= 5 and . &lt;= 9</t>
+  </si>
+  <si>
+    <t>The age must be between 5 and 9</t>
   </si>
   <si>
     <t>p_how_long</t>
@@ -1427,7 +1433,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1670,8 +1676,12 @@
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="15"/>
+      <c r="F9" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>41</v>
+      </c>
       <c r="H9" s="17" t="s">
         <v>37</v>
       </c>
@@ -1688,18 +1698,18 @@
         <v>14</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H10" s="17" t="s">
         <v>37</v>
@@ -1714,13 +1724,13 @@
     </row>
     <row r="11" s="3" customFormat="1" spans="1:13">
       <c r="A11" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -1742,17 +1752,17 @@
         <v>14</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="17"/>
       <c r="G12" s="15"/>
       <c r="H12" s="17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I12" s="15"/>
       <c r="J12" s="15" t="s">
@@ -1777,22 +1787,22 @@
     </row>
     <row r="14" s="3" customFormat="1" spans="1:13">
       <c r="A14" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="15"/>
       <c r="H14" s="17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
@@ -1802,17 +1812,17 @@
     </row>
     <row r="15" s="3" customFormat="1" spans="1:13">
       <c r="A15" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="15"/>
@@ -1830,18 +1840,18 @@
         <v>14</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H16" s="17"/>
       <c r="I16" s="15"/>
@@ -1854,7 +1864,7 @@
     </row>
     <row r="17" s="3" customFormat="1" spans="1:13">
       <c r="A17" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B17" s="15"/>
       <c r="D17" s="15"/>
@@ -1883,13 +1893,13 @@
     </row>
     <row r="19" s="3" customFormat="1" spans="1:13">
       <c r="A19" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -1908,20 +1918,20 @@
     </row>
     <row r="20" s="3" customFormat="1" ht="28.5" spans="1:13">
       <c r="A20" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="17"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I20" s="15"/>
       <c r="J20" s="15" t="s">
@@ -1936,17 +1946,17 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="17"/>
       <c r="G21" s="15"/>
       <c r="H21" s="15" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I21" s="15"/>
       <c r="J21" s="15" t="s">
@@ -1961,20 +1971,20 @@
     </row>
     <row r="22" s="3" customFormat="1" ht="42.75" spans="1:13">
       <c r="A22" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="17"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
@@ -1984,13 +1994,13 @@
     </row>
     <row r="23" s="3" customFormat="1" spans="1:13">
       <c r="A23" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
@@ -2004,10 +2014,10 @@
     </row>
     <row r="24" s="3" customFormat="1" spans="1:13">
       <c r="A24" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
@@ -2022,10 +2032,10 @@
     </row>
     <row r="25" s="3" customFormat="1" spans="1:13">
       <c r="A25" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
@@ -2075,93 +2085,93 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E1" s="12"/>
     </row>
     <row r="2" s="4" customFormat="1" spans="1:5">
       <c r="A2" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="13"/>
     </row>
     <row r="3" s="4" customFormat="1" spans="1:5">
       <c r="A3" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="13"/>
     </row>
     <row r="4" s="4" customFormat="1" spans="1:5">
       <c r="A4" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="13"/>
     </row>
     <row r="5" s="4" customFormat="1" spans="1:5">
       <c r="A5" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="13"/>
     </row>
     <row r="6" s="4" customFormat="1" spans="1:5">
       <c r="A6" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="13"/>
     </row>
     <row r="7" s="4" customFormat="1" spans="1:5">
       <c r="A7" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="13"/>
@@ -2175,26 +2185,26 @@
     </row>
     <row r="9" s="4" customFormat="1" spans="1:5">
       <c r="A9" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="13"/>
     </row>
     <row r="10" s="4" customFormat="1" spans="1:5">
       <c r="A10" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="13"/>
@@ -2208,156 +2218,156 @@
     </row>
     <row r="12" s="4" customFormat="1" spans="1:5">
       <c r="A12" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="13"/>
     </row>
     <row r="13" s="4" customFormat="1" spans="1:5">
       <c r="A13" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="13"/>
     </row>
     <row r="14" s="4" customFormat="1" spans="1:5">
       <c r="A14" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="13"/>
     </row>
     <row r="15" s="4" customFormat="1" spans="1:5">
       <c r="A15" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="13"/>
     </row>
     <row r="16" s="4" customFormat="1" spans="1:5">
       <c r="A16" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="13"/>
     </row>
     <row r="17" s="4" customFormat="1" spans="1:5">
       <c r="A17" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="13"/>
     </row>
     <row r="18" s="4" customFormat="1" spans="1:5">
       <c r="A18" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="13"/>
     </row>
     <row r="19" s="4" customFormat="1" spans="1:5">
       <c r="A19" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="13"/>
     </row>
     <row r="20" s="4" customFormat="1" spans="1:5">
       <c r="A20" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="13"/>
     </row>
     <row r="21" s="4" customFormat="1" spans="1:5">
       <c r="A21" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="13"/>
     </row>
     <row r="22" s="4" customFormat="1" spans="1:5">
       <c r="A22" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="13"/>
     </row>
     <row r="23" s="4" customFormat="1" spans="1:5">
       <c r="A23" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="13"/>
@@ -2550,24 +2560,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lr: updates oncho ias forms
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Liberia/lr_oncho_ias_2_participant_202112.xlsx
+++ b/ONCHO/Impact Assessments/Liberia/lr_oncho_ias_2_participant_202112.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12345" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="118">
   <si>
     <t>type</t>
   </si>
@@ -279,9 +279,6 @@
     <t>list_name</t>
   </si>
   <si>
-    <t>label</t>
-  </si>
-  <si>
     <t>region_list</t>
   </si>
   <si>
@@ -369,7 +366,7 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(Dec 2021) IAS - 2. Participant Form V2</t>
+    <t>(July 2022) IAS - 2. Participant Form V2</t>
   </si>
   <si>
     <t>lr_oncho_ias_2_participant_202112_v2</t>
@@ -380,10 +377,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -425,6 +422,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -432,18 +437,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -455,16 +453,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -477,17 +475,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -495,9 +484,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -516,14 +513,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -532,7 +521,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -546,21 +557,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -583,13 +580,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -601,91 +736,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -697,73 +760,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -841,22 +838,42 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -877,36 +894,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -922,145 +919,145 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2072,7 +2069,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="4"/>
@@ -2091,87 +2088,87 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="E1" s="12"/>
     </row>
     <row r="2" s="4" customFormat="1" spans="1:5">
       <c r="A2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="C2" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="13"/>
     </row>
     <row r="3" s="4" customFormat="1" spans="1:5">
       <c r="A3" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="13"/>
     </row>
     <row r="4" s="4" customFormat="1" spans="1:5">
       <c r="A4" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>93</v>
-      </c>
       <c r="C4" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="13"/>
     </row>
     <row r="5" s="4" customFormat="1" spans="1:5">
       <c r="A5" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="13"/>
     </row>
     <row r="6" s="4" customFormat="1" spans="1:5">
       <c r="A6" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>96</v>
-      </c>
       <c r="C6" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="13"/>
     </row>
     <row r="7" s="4" customFormat="1" spans="1:5">
       <c r="A7" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="13"/>
@@ -2185,26 +2182,26 @@
     </row>
     <row r="9" s="4" customFormat="1" spans="1:5">
       <c r="A9" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>99</v>
-      </c>
       <c r="C9" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="13"/>
     </row>
     <row r="10" s="4" customFormat="1" spans="1:5">
       <c r="A10" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="13"/>
@@ -2218,156 +2215,156 @@
     </row>
     <row r="12" s="4" customFormat="1" spans="1:5">
       <c r="A12" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>102</v>
-      </c>
       <c r="C12" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="13"/>
     </row>
     <row r="13" s="4" customFormat="1" spans="1:5">
       <c r="A13" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="13"/>
     </row>
     <row r="14" s="4" customFormat="1" spans="1:5">
       <c r="A14" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="13"/>
     </row>
     <row r="15" s="4" customFormat="1" spans="1:5">
       <c r="A15" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="13"/>
     </row>
     <row r="16" s="4" customFormat="1" spans="1:5">
       <c r="A16" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="13"/>
     </row>
     <row r="17" s="4" customFormat="1" spans="1:5">
       <c r="A17" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="13"/>
     </row>
     <row r="18" s="4" customFormat="1" spans="1:5">
       <c r="A18" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="13"/>
     </row>
     <row r="19" s="4" customFormat="1" spans="1:5">
       <c r="A19" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="13"/>
     </row>
     <row r="20" s="4" customFormat="1" spans="1:5">
       <c r="A20" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="13"/>
     </row>
     <row r="21" s="4" customFormat="1" spans="1:5">
       <c r="A21" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="13"/>
     </row>
     <row r="22" s="4" customFormat="1" spans="1:5">
       <c r="A22" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="13"/>
     </row>
     <row r="23" s="4" customFormat="1" spans="1:5">
       <c r="A23" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="13"/>
@@ -2548,7 +2545,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -2560,24 +2557,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" t="s">
         <v>117</v>
       </c>
-      <c r="B2" t="s">
-        <v>118</v>
-      </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>